<commit_message>
document templates for altyn
</commit_message>
<xml_diff>
--- a/templates/billout_tpl.xlsx
+++ b/templates/billout_tpl.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -33,12 +33,6 @@
     <t>Сч. №</t>
   </si>
   <si>
-    <t>ИНН 7723444811</t>
-  </si>
-  <si>
-    <t>КПП 772301001</t>
-  </si>
-  <si>
     <t>Счёт на оплату № ${number} от ${date}</t>
   </si>
   <si>
@@ -47,10 +41,6 @@
   <si>
     <t>Покупатель
 (Заказчик):</t>
-  </si>
-  <si>
-    <t>ООО "ВИДЖИЭФ", ИНН 7723444811, КПП 772301001, 109044, Москва г, Крутицкий
-вал ул, дом No 16, офис 102, тел.: +7 (495) 180-28-28</t>
   </si>
   <si>
     <t>${customer}</t>
@@ -120,26 +110,35 @@
 </t>
   </si>
   <si>
-    <t>Руководитель __________________________ Сокровищук В.А.</t>
-  </si>
-  <si>
-    <t>Бухгалтер __________________________ Сокровищук В.А.</t>
-  </si>
-  <si>
-    <t>40701810800000006836</t>
-  </si>
-  <si>
     <t>30101810100000000716</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ООО «Алтын Финанс», ИНН 9705109660, КПП 770501001, 115184, г. Москва, ул. Большая Татарская, дом 7, пом. XXXVI, тел.: +7 (495) 120-56-73</t>
+  </si>
+  <si>
+    <t>ИНН 9705109660</t>
+  </si>
+  <si>
+    <t>КПП 770501001</t>
+  </si>
+  <si>
+    <t>40701810112250000008</t>
+  </si>
+  <si>
+    <t>Руководитель __________________________ Усманов Р. М.</t>
+  </si>
+  <si>
+    <t>Бухгалтер __________________________ Усманов Р. М.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +553,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -572,15 +634,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,63 +676,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,9 +691,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -732,7 +731,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -766,7 +765,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -801,10 +799,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -977,17 +974,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -997,268 +994,277 @@
     <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26">
+      <c r="E1" s="44">
         <v>44525716</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="E2" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="49"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48"/>
-    </row>
-    <row r="7" spans="1:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="E6" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" ht="6.75" customHeight="1">
+      <c r="A7" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" ht="9.75" customHeight="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="1:7" ht="35.25" customHeight="1" thickBot="1">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" ht="33" customHeight="1">
+      <c r="A10" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" customHeight="1">
+      <c r="A11" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-    </row>
-    <row r="8" spans="1:7" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-    </row>
-    <row r="9" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-    </row>
-    <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="52" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-    </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="45" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="E14" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="38" t="s">
+      <c r="F14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="8" t="s">
+      <c r="G14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" ht="54" customHeight="1" thickBot="1">
       <c r="A15" s="12">
         <v>1</v>
       </c>
-      <c r="B15" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="41"/>
+      <c r="B15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="21"/>
       <c r="D15" s="13">
         <v>1</v>
       </c>
       <c r="E15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75">
+      <c r="F17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="G17" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75">
+      <c r="F18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G18" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75">
+      <c r="F19" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="11" t="s">
+      <c r="G19" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="11" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="11" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" s="22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-    </row>
-    <row r="27" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="1:7" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
@@ -1269,15 +1275,6 @@
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1285,24 +1282,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>